<commit_message>
data set in text python file
</commit_message>
<xml_diff>
--- a/websiteanalyzer/templates/Excel/main.xlsx
+++ b/websiteanalyzer/templates/Excel/main.xlsx
@@ -448,144 +448,144 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>http://varanasikshetra.com/pahadiamandirsarovarandakhara.aspx</t>
+          <t>http://varanasikshetra.com/bheemchandi.aspx</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>varanasikshetra_com_pahadiamandirsarovarandakhara_aspx.html</t>
+          <t>varanasikshetra_com_bheemchandi_aspx.html</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>http://varanasikshetra.com/</t>
+          <t>http://varanasikshetra.com/kapildhara.aspx</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>varanasikshetra_com_.html</t>
+          <t>varanasikshetra_com_kapildhara_aspx.html</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>http://varanasikshetra.com/bheemchandi.aspx</t>
+          <t>http://varanasikshetra.com/rameshwarmahadevgallery.aspx</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>varanasikshetra_com_bheemchandi_aspx.html</t>
+          <t>varanasikshetra_com_rameshwarmahadevgallery_aspx.html</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>http://varanasikshetra.com/#myCarousel</t>
+          <t>http://varanasikshetra.com/panchpandava.aspx</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>varanasikshetra_com__myCarousel.html</t>
+          <t>varanasikshetra_com_panchpandava_aspx.html</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>http://varanasikshetra.com/kashipanchkoshiparikrama.aspx</t>
+          <t>http://varanasikshetra.com/dindaspur-harsos-jansa.aspx</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>varanasikshetra_com_kashipanchkoshiparikrama_aspx.html</t>
+          <t>varanasikshetra_com_dindaspur-harsos-jansa_aspx.html</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>http://varanasikshetra.com/bhairavtalab.aspx</t>
+          <t>http://varanasikshetra.com/pahadiamandirsarovarandakhara.aspx</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>varanasikshetra_com_bhairavtalab_aspx.html</t>
+          <t>varanasikshetra_com_pahadiamandirsarovarandakhara_aspx.html</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>http://varanasikshetra.com/#myPage</t>
+          <t>http://varanasikshetra.com/kardameshwarmahadev.aspx</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>varanasikshetra_com__myPage.html</t>
+          <t>varanasikshetra_com_kardameshwarmahadev_aspx.html</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>http://varanasikshetra.com/kardameshwarmahadev.aspx</t>
+          <t>http://varanasikshetra.com/#myCarousel</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>varanasikshetra_com_kardameshwarmahadev_aspx.html</t>
+          <t>varanasikshetra_com__myCarousel.html</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>http://varanasikshetra.com/bheemchandigallery.aspx</t>
+          <t>http://varanasikshetra.com/kashipanchkoshiparikrama.aspx</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>varanasikshetra_com_bheemchandigallery_aspx.html</t>
+          <t>varanasikshetra_com_kashipanchkoshiparikrama_aspx.html</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>http://varanasikshetra.com/rameshwarmahadev.aspx</t>
+          <t>http://varanasikshetra.com/</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>varanasikshetra_com_rameshwarmahadev_aspx.html</t>
+          <t>varanasikshetra_com_.html</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>http://varanasikshetra.com/rameshwarmahadevgallery.aspx</t>
+          <t>http://varanasikshetra.com/bheemchandigallery.aspx</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>varanasikshetra_com_rameshwarmahadevgallery_aspx.html</t>
+          <t>varanasikshetra_com_bheemchandigallery_aspx.html</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>http://varanasikshetra.com/kapildharagallery.aspx</t>
+          <t>http://varanasikshetra.com/adikeshava.aspx</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>varanasikshetra_com_kapildharagallery_aspx.html</t>
+          <t>varanasikshetra_com_adikeshava_aspx.html</t>
         </is>
       </c>
     </row>
@@ -604,60 +604,60 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>http://varanasikshetra.com/kapildhara.aspx</t>
+          <t>http://varanasikshetra.com/rameshwarmahadev.aspx</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>varanasikshetra_com_kapildhara_aspx.html</t>
+          <t>varanasikshetra_com_rameshwarmahadev_aspx.html</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>http://varanasikshetra.com/panchpandava.aspx</t>
+          <t>http://varanasikshetra.com/bhairavtalab.aspx</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>varanasikshetra_com_panchpandava_aspx.html</t>
+          <t>varanasikshetra_com_bhairavtalab_aspx.html</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>http://varanasikshetra.com/dindaspur-harsos-jansa.aspx</t>
+          <t>http://varanasikshetra.com/index.aspx</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>varanasikshetra_com_dindaspur-harsos-jansa_aspx.html</t>
+          <t>varanasikshetra_com_index_aspx.html</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>http://varanasikshetra.com/adikeshava.aspx</t>
+          <t>http://varanasikshetra.com/kapildharagallery.aspx</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>varanasikshetra_com_adikeshava_aspx.html</t>
+          <t>varanasikshetra_com_kapildharagallery_aspx.html</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>http://varanasikshetra.com/index.aspx</t>
+          <t>http://varanasikshetra.com/#myPage</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>varanasikshetra_com_index_aspx.html</t>
+          <t>varanasikshetra_com__myPage.html</t>
         </is>
       </c>
     </row>

</xml_diff>